<commit_message>
EPBDS-7029 Add possibility to define values of arrays in test/data tables using several rows for a single test case/data object. Fix bug.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/MultiRowDatatableAndTests.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/MultiRowDatatableAndTests.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-7029\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605"/>
+    <workbookView windowHeight="10605" windowWidth="20100" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="62">
   <si>
     <t>Test lengthOf test2</t>
   </si>
@@ -189,12 +189,31 @@
   </si>
   <si>
     <t>x.beansB[].beansC[].name</t>
+  </si>
+  <si>
+    <t>Method int beansTest(BeanA x, BeanA y)</t>
+  </si>
+  <si>
+    <t>return lengthOf(x.beansB) +lengthOf(y.beansB);</t>
+  </si>
+  <si>
+    <t>y.beansB[].name</t>
+  </si>
+  <si>
+    <t>y.beansB[].beansC[].name</t>
+  </si>
+  <si>
+    <t>y.beansB[].beansC[].value</t>
+  </si>
+  <si>
+    <t>Test beansTest BeansTest2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -239,13 +258,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFFF" theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor rgb="4BACC6" theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,7 +276,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="F79646" theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,37 +300,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
+        <fgColor rgb="EEECE1" theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="8064A2" theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="C0504D" theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="C0504D" theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
+        <fgColor rgb="FFFFFF" theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF" theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,163 +500,203 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2"/>
   </cellStyleXfs>
-  <cellXfs count="60">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="74">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="3" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
+    <xf applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
+    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
+    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
+    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="7" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="8" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="10" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="13" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="11" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="9" fillId="14" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="14" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="8" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="10" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="7" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="13" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="6" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="11" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="14" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="14" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="13" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="14" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="12" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="5" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="9" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="9" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyFont="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="3" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="15" fillId="14" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="9" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="2">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="2">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent1 2" xfId="2"/>
+    <cellStyle name="20% - Accent1 2" xfId="0"/>
     <cellStyle name="Comma 2" xfId="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -654,10 +713,10 @@
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -692,7 +751,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -744,7 +803,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -849,7 +908,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -858,13 +917,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -874,7 +933,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -883,7 +942,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -892,7 +951,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -902,12 +961,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -938,7 +997,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -957,7 +1016,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -969,20 +1028,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:M130"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:N148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="E136" workbookViewId="0">
+      <selection activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="53.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="53.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="45.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -1006,13 +1067,13 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1064,7 +1125,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="63" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -1085,7 +1146,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="22" t="s">
         <v>1</v>
       </c>
@@ -1104,11 +1165,11 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="51"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="60" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="24" t="s">
@@ -1123,11 +1184,11 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="42"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="31" t="s">
         <v>1</v>
       </c>
@@ -1140,10 +1201,10 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="53">
-        <v>2</v>
-      </c>
-      <c r="C14" s="39" t="s">
+      <c r="B14" s="55">
+        <v>2</v>
+      </c>
+      <c r="C14" s="65" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="23" t="s">
@@ -1161,8 +1222,8 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="53"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="34" t="s">
         <v>9</v>
       </c>
@@ -1205,13 +1266,13 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="62"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1263,7 +1324,7 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="63" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="22" t="s">
@@ -1284,7 +1345,7 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="51"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="22" t="s">
         <v>1</v>
       </c>
@@ -1303,11 +1364,11 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="51"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="60" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -1322,11 +1383,11 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="51"/>
+      <c r="B24" s="63"/>
       <c r="C24" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="42"/>
+      <c r="D24" s="60"/>
       <c r="E24" s="31" t="s">
         <v>1</v>
       </c>
@@ -1339,10 +1400,10 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="53">
-        <v>2</v>
-      </c>
-      <c r="C25" s="39" t="s">
+      <c r="B25" s="55">
+        <v>2</v>
+      </c>
+      <c r="C25" s="65" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="23" t="s">
@@ -1360,8 +1421,8 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="53"/>
-      <c r="C26" s="39"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="65"/>
       <c r="D26" s="34" t="s">
         <v>9</v>
       </c>
@@ -1452,10 +1513,10 @@
       <c r="J35" s="1"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="50"/>
+      <c r="C38" s="62"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
@@ -1504,10 +1565,10 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="52"/>
+      <c r="C47" s="64"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
@@ -1556,10 +1617,10 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="52"/>
+      <c r="C55" s="64"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
@@ -1600,11 +1661,11 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="40" t="s">
+      <c r="B62" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C62" s="40"/>
-      <c r="D62" s="46"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="57"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1679,11 +1740,11 @@
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40"/>
+      <c r="C73" s="56"/>
+      <c r="D73" s="56"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
@@ -1742,10 +1803,10 @@
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="40" t="s">
+      <c r="B81" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C81" s="40"/>
+      <c r="C81" s="56"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
@@ -1794,10 +1855,10 @@
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="40" t="s">
+      <c r="B89" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C89" s="40"/>
+      <c r="C89" s="56"/>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -1846,10 +1907,10 @@
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="40" t="s">
+      <c r="B97" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C97" s="40"/>
+      <c r="C97" s="56"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
@@ -1890,13 +1951,13 @@
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="44" t="s">
+      <c r="B105" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C105" s="44"/>
-      <c r="D105" s="44"/>
-      <c r="E105" s="45"/>
-      <c r="F105" s="45"/>
+      <c r="C105" s="49"/>
+      <c r="D105" s="49"/>
+      <c r="E105" s="50"/>
+      <c r="F105" s="50"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
@@ -1931,7 +1992,7 @@
       <c r="F107" s="4"/>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B108" s="38" t="s">
+      <c r="B108" s="67" t="s">
         <v>9</v>
       </c>
       <c r="C108" s="23" t="s">
@@ -1943,12 +2004,12 @@
       <c r="E108" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F108" s="59">
+      <c r="F108" s="66">
         <v>2</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B109" s="38"/>
+      <c r="B109" s="67"/>
       <c r="C109" s="23" t="s">
         <v>9</v>
       </c>
@@ -1958,11 +2019,11 @@
       <c r="E109" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F109" s="59"/>
+      <c r="F109" s="66"/>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B110" s="38"/>
-      <c r="C110" s="42" t="s">
+      <c r="B110" s="67"/>
+      <c r="C110" s="60" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="24" t="s">
@@ -1971,21 +2032,21 @@
       <c r="E110" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F110" s="59"/>
+      <c r="F110" s="66"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B111" s="38"/>
-      <c r="C111" s="43"/>
+      <c r="B111" s="67"/>
+      <c r="C111" s="53"/>
       <c r="D111" s="31" t="s">
         <v>1</v>
       </c>
       <c r="E111" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F111" s="59"/>
+      <c r="F111" s="66"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="39" t="s">
+      <c r="B112" s="65" t="s">
         <v>9</v>
       </c>
       <c r="C112" s="23" t="s">
@@ -1997,12 +2058,12 @@
       <c r="E112" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F112" s="59">
+      <c r="F112" s="66">
         <v>2</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B113" s="41"/>
+      <c r="B113" s="68"/>
       <c r="C113" s="34" t="s">
         <v>9</v>
       </c>
@@ -2012,7 +2073,7 @@
       <c r="E113" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F113" s="59"/>
+      <c r="F113" s="66"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="8" t="s">
@@ -2032,13 +2093,13 @@
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="44" t="s">
+      <c r="B118" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="C118" s="44"/>
-      <c r="D118" s="44"/>
-      <c r="E118" s="45"/>
-      <c r="F118" s="45"/>
+      <c r="C118" s="49"/>
+      <c r="D118" s="49"/>
+      <c r="E118" s="50"/>
+      <c r="F118" s="50"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
@@ -2073,7 +2134,7 @@
       <c r="F120" s="4"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="38" t="s">
+      <c r="B121" s="67" t="s">
         <v>9</v>
       </c>
       <c r="C121" s="23" t="s">
@@ -2085,12 +2146,12 @@
       <c r="E121" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F121" s="59">
+      <c r="F121" s="66">
         <v>2</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="38"/>
+      <c r="B122" s="67"/>
       <c r="C122" s="23" t="s">
         <v>9</v>
       </c>
@@ -2100,11 +2161,11 @@
       <c r="E122" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F122" s="59"/>
+      <c r="F122" s="66"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="38"/>
-      <c r="C123" s="42" t="s">
+      <c r="B123" s="67"/>
+      <c r="C123" s="60" t="s">
         <v>8</v>
       </c>
       <c r="D123" s="24" t="s">
@@ -2113,21 +2174,21 @@
       <c r="E123" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F123" s="59"/>
+      <c r="F123" s="66"/>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B124" s="38"/>
-      <c r="C124" s="43"/>
+      <c r="B124" s="67"/>
+      <c r="C124" s="53"/>
       <c r="D124" s="31" t="s">
         <v>1</v>
       </c>
       <c r="E124" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F124" s="59"/>
+      <c r="F124" s="66"/>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B125" s="39" t="s">
+      <c r="B125" s="65" t="s">
         <v>9</v>
       </c>
       <c r="C125" s="23" t="s">
@@ -2139,12 +2200,12 @@
       <c r="E125" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F125" s="59">
+      <c r="F125" s="66">
         <v>2</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="41"/>
+      <c r="B126" s="68"/>
       <c r="C126" s="34" t="s">
         <v>9</v>
       </c>
@@ -2154,7 +2215,7 @@
       <c r="E126" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F126" s="59"/>
+      <c r="F126" s="66"/>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="8" t="s">
@@ -2173,18 +2234,224 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="11" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B132" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B133" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B139" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C139" s="49"/>
+      <c r="D139" s="49"/>
+      <c r="E139" s="49"/>
+      <c r="F139" s="49"/>
+      <c r="G139" s="49"/>
+      <c r="H139" s="49"/>
+      <c r="I139" s="50"/>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B140" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C140" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D140" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E140" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="F140" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="G140" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="H140" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="I140" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B141" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D141" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E141" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F141" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G141" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H141" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="I141" s="4"/>
+    </row>
+    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B142" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E142" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F142" s="46"/>
+      <c r="G142" s="46"/>
+      <c r="H142" s="46"/>
+      <c r="I142" s="47" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B143" s="51"/>
+      <c r="C143" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E143" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="F143" s="46"/>
+      <c r="G143" s="46"/>
+      <c r="H143" s="46"/>
+      <c r="I143" s="47"/>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B144" s="51"/>
+      <c r="C144" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F144" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G144" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="H144" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I144" s="47"/>
+    </row>
+    <row r="145" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B145" s="51"/>
+      <c r="C145" s="53"/>
+      <c r="D145" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E145" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F145" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G145" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="H145" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="I145" s="47"/>
+    </row>
+    <row r="146" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B146" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C146" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D146" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F146" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="G146" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="H146" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="I146" s="47" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B147" s="55"/>
+      <c r="C147" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D147" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F147" s="46"/>
+      <c r="G147" s="46"/>
+      <c r="H147" s="46"/>
+      <c r="I147" s="47"/>
+    </row>
+    <row r="148" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B148" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+      <c r="F148" s="8"/>
+      <c r="G148" s="8"/>
+      <c r="H148" s="8"/>
+      <c r="I148" s="38" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="36">
     <mergeCell ref="F121:F124"/>
     <mergeCell ref="F125:F126"/>
     <mergeCell ref="B105:F105"/>
@@ -2196,12 +2463,7 @@
     <mergeCell ref="B125:B126"/>
     <mergeCell ref="C123:C124"/>
     <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B121:B124"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B38:C38"/>
@@ -2209,20 +2471,31 @@
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B121:B124"/>
     <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="D23:D24"/>
     <mergeCell ref="B73:D73"/>
     <mergeCell ref="B81:C81"/>
     <mergeCell ref="B89:C89"/>
     <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="I142:I145"/>
+    <mergeCell ref="I146:I147"/>
+    <mergeCell ref="B139:I139"/>
+    <mergeCell ref="B142:B145"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="B146:B147"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
@@ -2231,10 +2504,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="73"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
@@ -2253,10 +2526,10 @@
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="55"/>
+      <c r="C9" s="70"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
@@ -2275,10 +2548,10 @@
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="72"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
@@ -2302,18 +2575,18 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-7224 Wrong assignment of values for objects-elements of an array in case of empty cells
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/MultiRowDatatableAndTests.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/MultiRowDatatableAndTests.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-7029\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="10605" windowWidth="20100" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="62">
   <si>
     <t>Test lengthOf test2</t>
   </si>
@@ -213,7 +213,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -258,13 +257,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF" theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="4BACC6" theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +275,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="F79646" theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,37 +299,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="EEECE1" theme="2" tint="-0.499984740745262"/>
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="8064A2" theme="7"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="C0504D" theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="C0504D" theme="5"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF" theme="0" tint="-0.499984740745262"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF" theme="0"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,203 +499,203 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="74">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="3" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="7" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="8" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="10" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="13" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="11" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="9" fillId="14" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="14" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="8" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="10" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="7" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="13" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="6" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="11" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="14" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="14" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="13" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="14" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="12" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="5" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="9" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="9" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="3" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="15" fillId="14" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="9" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="2">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="2">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent1 2" xfId="0"/>
+    <cellStyle name="20% - Accent1 2" xfId="2"/>
     <cellStyle name="Comma 2" xfId="1"/>
-    <cellStyle builtinId="0" name="Обычный" xfId="2"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -713,10 +712,10 @@
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -751,7 +750,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -803,7 +802,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -908,7 +907,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -917,13 +916,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -933,7 +932,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -942,7 +941,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -951,7 +950,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -961,12 +960,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -997,7 +996,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1016,7 +1015,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1028,22 +1027,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:N148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:M148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E136" workbookViewId="0">
-      <selection activeCell="G157" sqref="G157"/>
+      <selection activeCell="J149" sqref="J149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="40.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="53.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="45.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="41.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="41.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="39.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -1067,13 +1066,13 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1125,7 +1124,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="58" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -1146,7 +1145,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="63"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="22" t="s">
         <v>1</v>
       </c>
@@ -1165,11 +1164,11 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="63"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="51" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="24" t="s">
@@ -1184,11 +1183,11 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="63"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="51"/>
       <c r="E13" s="31" t="s">
         <v>1</v>
       </c>
@@ -1201,10 +1200,10 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="55">
-        <v>2</v>
-      </c>
-      <c r="C14" s="65" t="s">
+      <c r="B14" s="59">
+        <v>2</v>
+      </c>
+      <c r="C14" s="53" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="23" t="s">
@@ -1222,8 +1221,8 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="55"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="34" t="s">
         <v>9</v>
       </c>
@@ -1266,13 +1265,13 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="57"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1324,7 +1323,7 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="58" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="22" t="s">
@@ -1345,7 +1344,7 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="63"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="22" t="s">
         <v>1</v>
       </c>
@@ -1364,11 +1363,11 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="63"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="51" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -1383,11 +1382,11 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="63"/>
+      <c r="B24" s="58"/>
       <c r="C24" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="60"/>
+      <c r="D24" s="51"/>
       <c r="E24" s="31" t="s">
         <v>1</v>
       </c>
@@ -1400,10 +1399,10 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="55">
-        <v>2</v>
-      </c>
-      <c r="C25" s="65" t="s">
+      <c r="B25" s="59">
+        <v>2</v>
+      </c>
+      <c r="C25" s="53" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="23" t="s">
@@ -1421,8 +1420,8 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="55"/>
-      <c r="C26" s="65"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="34" t="s">
         <v>9</v>
       </c>
@@ -1513,10 +1512,10 @@
       <c r="J35" s="1"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="62"/>
+      <c r="C38" s="57"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
@@ -1565,10 +1564,10 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="64"/>
+      <c r="C47" s="56"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
@@ -1617,10 +1616,10 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="64"/>
+      <c r="C55" s="56"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
@@ -1661,11 +1660,11 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="56" t="s">
+      <c r="B62" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C62" s="56"/>
-      <c r="D62" s="57"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="63"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1740,11 +1739,11 @@
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="56" t="s">
+      <c r="B73" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="C73" s="56"/>
-      <c r="D73" s="56"/>
+      <c r="C73" s="55"/>
+      <c r="D73" s="55"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
@@ -1803,10 +1802,10 @@
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="56" t="s">
+      <c r="B81" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C81" s="56"/>
+      <c r="C81" s="55"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
@@ -1855,10 +1854,10 @@
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="56" t="s">
+      <c r="B89" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C89" s="56"/>
+      <c r="C89" s="55"/>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -1907,10 +1906,10 @@
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="56" t="s">
+      <c r="B97" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C97" s="56"/>
+      <c r="C97" s="55"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
@@ -1951,13 +1950,13 @@
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="49" t="s">
+      <c r="B105" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C105" s="49"/>
-      <c r="D105" s="49"/>
-      <c r="E105" s="50"/>
-      <c r="F105" s="50"/>
+      <c r="C105" s="48"/>
+      <c r="D105" s="48"/>
+      <c r="E105" s="49"/>
+      <c r="F105" s="49"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
@@ -1992,7 +1991,7 @@
       <c r="F107" s="4"/>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B108" s="67" t="s">
+      <c r="B108" s="50" t="s">
         <v>9</v>
       </c>
       <c r="C108" s="23" t="s">
@@ -2004,12 +2003,12 @@
       <c r="E108" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F108" s="66">
+      <c r="F108" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B109" s="67"/>
+      <c r="B109" s="50"/>
       <c r="C109" s="23" t="s">
         <v>9</v>
       </c>
@@ -2019,11 +2018,11 @@
       <c r="E109" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F109" s="66"/>
+      <c r="F109" s="47"/>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B110" s="67"/>
-      <c r="C110" s="60" t="s">
+      <c r="B110" s="50"/>
+      <c r="C110" s="51" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="24" t="s">
@@ -2032,21 +2031,21 @@
       <c r="E110" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F110" s="66"/>
+      <c r="F110" s="47"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B111" s="67"/>
-      <c r="C111" s="53"/>
+      <c r="B111" s="50"/>
+      <c r="C111" s="52"/>
       <c r="D111" s="31" t="s">
         <v>1</v>
       </c>
       <c r="E111" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F111" s="66"/>
+      <c r="F111" s="47"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="65" t="s">
+      <c r="B112" s="53" t="s">
         <v>9</v>
       </c>
       <c r="C112" s="23" t="s">
@@ -2058,12 +2057,12 @@
       <c r="E112" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F112" s="66">
+      <c r="F112" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B113" s="68"/>
+      <c r="B113" s="54"/>
       <c r="C113" s="34" t="s">
         <v>9</v>
       </c>
@@ -2073,7 +2072,7 @@
       <c r="E113" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F113" s="66"/>
+      <c r="F113" s="47"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="8" t="s">
@@ -2093,13 +2092,13 @@
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="49" t="s">
+      <c r="B118" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C118" s="49"/>
-      <c r="D118" s="49"/>
-      <c r="E118" s="50"/>
-      <c r="F118" s="50"/>
+      <c r="C118" s="48"/>
+      <c r="D118" s="48"/>
+      <c r="E118" s="49"/>
+      <c r="F118" s="49"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
@@ -2134,7 +2133,7 @@
       <c r="F120" s="4"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="67" t="s">
+      <c r="B121" s="50" t="s">
         <v>9</v>
       </c>
       <c r="C121" s="23" t="s">
@@ -2146,12 +2145,12 @@
       <c r="E121" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F121" s="66">
+      <c r="F121" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="67"/>
+      <c r="B122" s="50"/>
       <c r="C122" s="23" t="s">
         <v>9</v>
       </c>
@@ -2161,11 +2160,11 @@
       <c r="E122" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F122" s="66"/>
+      <c r="F122" s="47"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="67"/>
-      <c r="C123" s="60" t="s">
+      <c r="B123" s="50"/>
+      <c r="C123" s="51" t="s">
         <v>8</v>
       </c>
       <c r="D123" s="24" t="s">
@@ -2174,21 +2173,21 @@
       <c r="E123" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F123" s="66"/>
+      <c r="F123" s="47"/>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B124" s="67"/>
-      <c r="C124" s="53"/>
+      <c r="B124" s="50"/>
+      <c r="C124" s="52"/>
       <c r="D124" s="31" t="s">
         <v>1</v>
       </c>
       <c r="E124" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F124" s="66"/>
+      <c r="F124" s="47"/>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B125" s="65" t="s">
+      <c r="B125" s="53" t="s">
         <v>9</v>
       </c>
       <c r="C125" s="23" t="s">
@@ -2200,12 +2199,12 @@
       <c r="E125" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F125" s="66">
+      <c r="F125" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="68"/>
+      <c r="B126" s="54"/>
       <c r="C126" s="34" t="s">
         <v>9</v>
       </c>
@@ -2215,7 +2214,7 @@
       <c r="E126" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F126" s="66"/>
+      <c r="F126" s="47"/>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="8" t="s">
@@ -2255,16 +2254,16 @@
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B139" s="48" t="s">
+      <c r="B139" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="C139" s="49"/>
-      <c r="D139" s="49"/>
-      <c r="E139" s="49"/>
-      <c r="F139" s="49"/>
-      <c r="G139" s="49"/>
-      <c r="H139" s="49"/>
-      <c r="I139" s="50"/>
+      <c r="C139" s="48"/>
+      <c r="D139" s="48"/>
+      <c r="E139" s="48"/>
+      <c r="F139" s="48"/>
+      <c r="G139" s="48"/>
+      <c r="H139" s="48"/>
+      <c r="I139" s="49"/>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" s="2" t="s">
@@ -2317,7 +2316,7 @@
       <c r="I141" s="4"/>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B142" s="51" t="s">
+      <c r="B142" s="66" t="s">
         <v>9</v>
       </c>
       <c r="C142" s="44" t="s">
@@ -2332,12 +2331,12 @@
       <c r="F142" s="46"/>
       <c r="G142" s="46"/>
       <c r="H142" s="46"/>
-      <c r="I142" s="47" t="n">
-        <v>3.0</v>
+      <c r="I142" s="64">
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B143" s="51"/>
+      <c r="B143" s="66"/>
       <c r="C143" s="44" t="s">
         <v>9</v>
       </c>
@@ -2350,11 +2349,11 @@
       <c r="F143" s="46"/>
       <c r="G143" s="46"/>
       <c r="H143" s="46"/>
-      <c r="I143" s="47"/>
+      <c r="I143" s="64"/>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B144" s="51"/>
-      <c r="C144" s="52" t="s">
+      <c r="B144" s="66"/>
+      <c r="C144" s="67" t="s">
         <v>8</v>
       </c>
       <c r="D144" s="42" t="s">
@@ -2372,11 +2371,11 @@
       <c r="H144" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I144" s="47"/>
+      <c r="I144" s="64"/>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B145" s="51"/>
-      <c r="C145" s="53"/>
+      <c r="B145" s="66"/>
+      <c r="C145" s="52"/>
       <c r="D145" s="43" t="s">
         <v>1</v>
       </c>
@@ -2392,10 +2391,10 @@
       <c r="H145" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="I145" s="47"/>
+      <c r="I145" s="64"/>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B146" s="54" t="s">
+      <c r="B146" s="68" t="s">
         <v>9</v>
       </c>
       <c r="C146" s="44" t="s">
@@ -2416,12 +2415,12 @@
       <c r="H146" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I146" s="47" t="n">
-        <v>3.0</v>
+      <c r="I146" s="64">
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B147" s="55"/>
+      <c r="B147" s="59"/>
       <c r="C147" s="45" t="s">
         <v>9</v>
       </c>
@@ -2434,7 +2433,7 @@
       <c r="F147" s="46"/>
       <c r="G147" s="46"/>
       <c r="H147" s="46"/>
-      <c r="I147" s="47"/>
+      <c r="I147" s="64"/>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B148" s="7" t="s">
@@ -2446,12 +2445,36 @@
       <c r="F148" s="8"/>
       <c r="G148" s="8"/>
       <c r="H148" s="8"/>
-      <c r="I148" s="38" t="n">
-        <v>0.0</v>
+      <c r="I148" s="38">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="I142:I145"/>
+    <mergeCell ref="I146:I147"/>
+    <mergeCell ref="B139:I139"/>
+    <mergeCell ref="B142:B145"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
     <mergeCell ref="F121:F124"/>
     <mergeCell ref="F125:F126"/>
     <mergeCell ref="B105:F105"/>
@@ -2464,38 +2487,14 @@
     <mergeCell ref="C123:C124"/>
     <mergeCell ref="B118:F118"/>
     <mergeCell ref="B121:B124"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="I142:I145"/>
-    <mergeCell ref="I146:I147"/>
-    <mergeCell ref="B139:I139"/>
-    <mergeCell ref="B142:B145"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="B146:B147"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
@@ -2575,18 +2574,18 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-7029 Add possibility to define values of arrays in test/data tables using several rows for a single test case/data object
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/MultiRowDatatableAndTests.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/MultiRowDatatableAndTests.xlsx
@@ -53,160 +53,160 @@
     <t>y</t>
   </si>
   <si>
+    <t>return length(x);</t>
+  </si>
+  <si>
+    <t>Datatype BeanA</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>BeanB[]</t>
+  </si>
+  <si>
+    <t>beansB</t>
+  </si>
+  <si>
+    <t>Datatype BeanB</t>
+  </si>
+  <si>
+    <t>beansC</t>
+  </si>
+  <si>
+    <t>BeanC[]</t>
+  </si>
+  <si>
+    <t>Datatype BeanC</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Data BeanA BeansA</t>
+  </si>
+  <si>
+    <t>&gt;  BeansA.beansB</t>
+  </si>
+  <si>
+    <t>Test lengthOf test1</t>
+  </si>
+  <si>
+    <t>&gt;  BeansA.beansB[0].beansC</t>
+  </si>
+  <si>
+    <t>Test lengthOf test3</t>
+  </si>
+  <si>
+    <t>&gt;  BeansA.beansB[1].beansC</t>
+  </si>
+  <si>
+    <t>Data BeanA BeansA2</t>
+  </si>
+  <si>
+    <t>Test eq test4</t>
+  </si>
+  <si>
+    <t>&gt;  BeansA.beansB[0].name</t>
+  </si>
+  <si>
+    <t>Method boolean eq(String x, String y)</t>
+  </si>
+  <si>
+    <t>return x == y;</t>
+  </si>
+  <si>
+    <t>Test eq test5</t>
+  </si>
+  <si>
+    <t>&gt;  BeansA2.beansB[0].name</t>
+  </si>
+  <si>
+    <t>Test lengthOf test6</t>
+  </si>
+  <si>
+    <t>&gt;  BeansA2.beansB</t>
+  </si>
+  <si>
+    <t>Test lengthOf test7</t>
+  </si>
+  <si>
+    <t>&gt;  BeansA2.beansB[0].beansC</t>
+  </si>
+  <si>
+    <t>Test lengthOf test8</t>
+  </si>
+  <si>
+    <t>&gt;  BeansA2.beansB[1].beansC</t>
+  </si>
+  <si>
+    <t>Test beanTest BeansA2Test</t>
+  </si>
+  <si>
+    <t>x.name</t>
+  </si>
+  <si>
+    <t>return lengthOf(x.beansB);</t>
+  </si>
+  <si>
+    <t>Method int beanTest(BeanA x)</t>
+  </si>
+  <si>
+    <t>Test beanTest BeansATest</t>
+  </si>
+  <si>
+    <t>Method int beansTest(BeanA x, BeanA y)</t>
+  </si>
+  <si>
+    <t>return lengthOf(x.beansB) +lengthOf(y.beansB);</t>
+  </si>
+  <si>
+    <t>Test beansTest BeansTest2</t>
+  </si>
+  <si>
+    <t>y.beansB.name</t>
+  </si>
+  <si>
+    <t>y.beansB.beansC.name</t>
+  </si>
+  <si>
+    <t>y.beansB.beansC.value</t>
+  </si>
+  <si>
+    <t>x.beansB.beansC.value</t>
+  </si>
+  <si>
+    <t>x.beansB.beansC.name</t>
+  </si>
+  <si>
+    <t>beansB.name</t>
+  </si>
+  <si>
+    <t>beansB.beansC.name</t>
+  </si>
+  <si>
+    <t>beansB.beansC.value</t>
+  </si>
+  <si>
+    <t>beansB._PK_</t>
+  </si>
+  <si>
+    <t>beansB.beansC._PK_</t>
+  </si>
+  <si>
+    <t>x.beansB.name</t>
+  </si>
+  <si>
+    <t>x.beansB._PK_</t>
+  </si>
+  <si>
+    <t>x.beansB.beansC._PK_</t>
+  </si>
+  <si>
     <t>Method int lengthOf(Object[] x)</t>
-  </si>
-  <si>
-    <t>return length(x);</t>
-  </si>
-  <si>
-    <t>Datatype BeanA</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>BeanB[]</t>
-  </si>
-  <si>
-    <t>beansB</t>
-  </si>
-  <si>
-    <t>Datatype BeanB</t>
-  </si>
-  <si>
-    <t>beansC</t>
-  </si>
-  <si>
-    <t>BeanC[]</t>
-  </si>
-  <si>
-    <t>beansB[].name</t>
-  </si>
-  <si>
-    <t>beansB[].beansC[].name</t>
-  </si>
-  <si>
-    <t>Datatype BeanC</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>beansB[].beansC[].value</t>
-  </si>
-  <si>
-    <t>Data BeanA BeansA</t>
-  </si>
-  <si>
-    <t>&gt;  BeansA.beansB</t>
-  </si>
-  <si>
-    <t>Test lengthOf test1</t>
-  </si>
-  <si>
-    <t>&gt;  BeansA.beansB[0].beansC</t>
-  </si>
-  <si>
-    <t>Test lengthOf test3</t>
-  </si>
-  <si>
-    <t>&gt;  BeansA.beansB[1].beansC</t>
-  </si>
-  <si>
-    <t>Data BeanA BeansA2</t>
-  </si>
-  <si>
-    <t>beansB[]._PK_</t>
-  </si>
-  <si>
-    <t>beansB[].beansC[]._PK_</t>
-  </si>
-  <si>
-    <t>Test eq test4</t>
-  </si>
-  <si>
-    <t>&gt;  BeansA.beansB[0].name</t>
-  </si>
-  <si>
-    <t>Method boolean eq(String x, String y)</t>
-  </si>
-  <si>
-    <t>return x == y;</t>
-  </si>
-  <si>
-    <t>Test eq test5</t>
-  </si>
-  <si>
-    <t>&gt;  BeansA2.beansB[0].name</t>
-  </si>
-  <si>
-    <t>Test lengthOf test6</t>
-  </si>
-  <si>
-    <t>&gt;  BeansA2.beansB</t>
-  </si>
-  <si>
-    <t>Test lengthOf test7</t>
-  </si>
-  <si>
-    <t>&gt;  BeansA2.beansB[0].beansC</t>
-  </si>
-  <si>
-    <t>Test lengthOf test8</t>
-  </si>
-  <si>
-    <t>&gt;  BeansA2.beansB[1].beansC</t>
-  </si>
-  <si>
-    <t>Test beanTest BeansA2Test</t>
-  </si>
-  <si>
-    <t>x.name</t>
-  </si>
-  <si>
-    <t>x.beansB[]._PK_</t>
-  </si>
-  <si>
-    <t>x.beansB[].beansC[]._PK_</t>
-  </si>
-  <si>
-    <t>x.beansB[].beansC[].value</t>
-  </si>
-  <si>
-    <t>return lengthOf(x.beansB);</t>
-  </si>
-  <si>
-    <t>Method int beanTest(BeanA x)</t>
-  </si>
-  <si>
-    <t>Test beanTest BeansATest</t>
-  </si>
-  <si>
-    <t>x.beansB[].name</t>
-  </si>
-  <si>
-    <t>x.beansB[].beansC[].name</t>
-  </si>
-  <si>
-    <t>Method int beansTest(BeanA x, BeanA y)</t>
-  </si>
-  <si>
-    <t>return lengthOf(x.beansB) +lengthOf(y.beansB);</t>
-  </si>
-  <si>
-    <t>y.beansB[].name</t>
-  </si>
-  <si>
-    <t>y.beansB[].beansC[].name</t>
-  </si>
-  <si>
-    <t>y.beansB[].beansC[].value</t>
-  </si>
-  <si>
-    <t>Test beansTest BeansTest2</t>
   </si>
 </sst>
 </file>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:M148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E136" workbookViewId="0">
-      <selection activeCell="J149" sqref="J149"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="60" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="61"/>
@@ -1086,16 +1086,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="55" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="62"/>
       <c r="D18" s="62"/>
@@ -1285,16 +1285,16 @@
         <v>3</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="55" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C38" s="57"/>
     </row>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C40" s="4"/>
     </row>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C49" s="4"/>
     </row>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="55" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C55" s="56"/>
     </row>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C57" s="4"/>
     </row>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="55" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C62" s="55"/>
       <c r="D62" s="63"/>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="4"/>
@@ -1730,17 +1730,17 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="55" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C73" s="55"/>
       <c r="D73" s="55"/>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="4"/>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="55" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C81" s="55"/>
     </row>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C83" s="4"/>
     </row>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="55" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C89" s="55"/>
     </row>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C91" s="4"/>
     </row>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="55" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C97" s="55"/>
     </row>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C99" s="4"/>
     </row>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="48" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C105" s="48"/>
       <c r="D105" s="48"/>
@@ -1960,16 +1960,16 @@
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F106" s="4" t="s">
         <v>2</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" s="48" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C118" s="48"/>
       <c r="D118" s="48"/>
@@ -2102,16 +2102,16 @@
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F119" s="4" t="s">
         <v>2</v>
@@ -2235,27 +2235,27 @@
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="10" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="11" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" s="10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" s="11" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B139" s="65" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C139" s="48"/>
       <c r="D139" s="48"/>
@@ -2267,25 +2267,25 @@
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C140" s="39" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D140" s="39" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E140" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F140" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G140" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H140" s="39" t="s">
         <v>50</v>
-      </c>
-      <c r="F140" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="G140" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="H140" s="39" t="s">
-        <v>60</v>
       </c>
       <c r="I140" s="4" t="s">
         <v>2</v>
@@ -2504,68 +2504,68 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="69" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="73"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="70"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="71" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="72"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>13</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>